<commit_message>
editing inaccurate fastq file names for the Rep3 samples
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_J.PLAGGENBERG_03.18.20.xlsx
+++ b/fastqFiles/fastq_J.PLAGGENBERG_03.18.20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF6C3B1-F63E-B040-9ACD-7D7FAB551AEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F65C5B-30A6-CF4D-B4CC-02195AD87B0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17680" yWindow="460" windowWidth="20920" windowHeight="19800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="460" windowWidth="34060" windowHeight="19800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="118">
   <si>
     <t>libraryDate</t>
   </si>
@@ -369,6 +369,24 @@
   </si>
   <si>
     <t>Brent/Brent_99_GTAC40_SIC_Index2_07_GTACGGCATC_GAGTTGGT_S101_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent/Brent_41_GTAC1_SIC_Index2_09_TGAGGTTATC_GACCTTGT_S42_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent/Brent_42_GTAC21_SIC_Index2_09_CTCAATGATC_TGTGAGGT_S43_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent/Brent_43_GTAC22_SIC_Index2_09_AAATGCAATC_TGTGAGGT_S44_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent/Brent_44_GTAC23_SIC_Index2_09_ACGCGGGATC_TGTGAGGT_S45_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent/Brent_45_GTAC24_SIC_Index2_09_GGAGTCCATC_TGTGAGGT_S46_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent/Brent_46_GTAC25_SIC_Index2_09_CGTCGCTATC_TGTGAGGT_S47_R1_001.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -864,15 +882,16 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="9" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="76.33203125" customWidth="1"/>
     <col min="13" max="1025" width="10.6640625" customWidth="1"/>
   </cols>
@@ -2376,7 +2395,7 @@
         <v>3341</v>
       </c>
       <c r="L42" s="12" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -2411,7 +2430,7 @@
         <v>3833001</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -2446,7 +2465,7 @@
         <v>2979687</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -2481,7 +2500,7 @@
         <v>3775249</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
@@ -2516,7 +2535,7 @@
         <v>2618801</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -2551,7 +2570,7 @@
         <v>4016231</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -2586,7 +2605,7 @@
         <v>5116059</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -2621,7 +2640,7 @@
         <v>3810168</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -2656,7 +2675,7 @@
         <v>3705711</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -2691,7 +2710,7 @@
         <v>5217361</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -2726,7 +2745,7 @@
         <v>3436627</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
@@ -2761,7 +2780,7 @@
         <v>3600852</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -2796,7 +2815,7 @@
         <v>405872</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -2831,7 +2850,7 @@
         <v>3996125</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -2866,7 +2885,7 @@
         <v>3411619</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
@@ -2901,7 +2920,7 @@
         <v>3249254</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -2936,7 +2955,7 @@
         <v>2678609</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
@@ -2971,7 +2990,7 @@
         <v>2459097</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
@@ -3006,7 +3025,7 @@
         <v>727852</v>
       </c>
       <c r="L60" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>